<commit_message>
AFDP-939: Adding default owning group to the assignment rules
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="535" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="535"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="ObjectTypes" vbProcedure="false">Sheet2!$A$2:$A$51</definedName>
-    <definedName function="false" hidden="false" name="ParticipantTypes" vbProcedure="false">Sheet2!$B$2:$B$51</definedName>
+    <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
+    <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>RuleSet</t>
   </si>
@@ -183,37 +182,33 @@
   <si>
     <t>ACCESS CONTROL LIST</t>
   </si>
+  <si>
+    <t>Complaint – Default group</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == 'owning group'].isEmpty()</t>
+  </si>
+  <si>
+    <t>Case File – Default group</t>
+  </si>
+  <si>
+    <t>owning group, ACM_INVESTIGATOR_DEV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -280,214 +275,217 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -546,35 +544,330 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="G22" activeCellId="0" pane="topLeft" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="56.42578125"/>
+    <col min="5" max="5" width="43.85546875"/>
+    <col min="6" max="6" width="30.5703125"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -584,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -594,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -604,7 +897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -614,7 +907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -624,7 +917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -634,7 +927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -644,7 +937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -654,7 +947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="225.5" outlineLevel="0" r="10">
+    <row r="10" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -664,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -674,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
@@ -685,7 +978,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -704,7 +997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -715,7 +1008,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10" t="s">
@@ -734,7 +1027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="17">
+    <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -757,7 +1050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="17" t="s">
         <v>28</v>
@@ -776,7 +1069,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>33</v>
@@ -793,7 +1086,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>36</v>
@@ -810,7 +1103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>39</v>
@@ -827,25 +1120,43 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
+      <c r="B22" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="G22" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="B23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="G23" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17"/>
       <c r="C24" s="19"/>
@@ -854,7 +1165,7 @@
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17"/>
       <c r="C25" s="19"/>
@@ -863,7 +1174,7 @@
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17"/>
       <c r="C26" s="19"/>
@@ -872,7 +1183,7 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17"/>
       <c r="C27" s="19"/>
@@ -881,7 +1192,7 @@
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17"/>
       <c r="C28" s="19"/>
@@ -890,7 +1201,7 @@
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17"/>
       <c r="C29" s="19"/>
@@ -900,106 +1211,83 @@
       <c r="G29" s="19"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="18.7109375"/>
+    <col min="2" max="2" width="17.5703125"/>
+    <col min="3" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AFDP-1050 - Implement Document level security - folder security - can set participants via the folder structure at case creation time, or via normal access control and assignment rules.
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>RuleSet</t>
   </si>
@@ -136,22 +136,25 @@
     <t>participants.?[participantType == 'assignee'].isEmpty()</t>
   </si>
   <si>
+    <t>assignee, samuel-acm</t>
+  </si>
+  <si>
+    <t>Complaint – Default access</t>
+  </si>
+  <si>
+    <t>participants.?[participantType == '*'].isEmpty()</t>
+  </si>
+  <si>
+    <t>*, *</t>
+  </si>
+  <si>
+    <t>Case File – Default assignee</t>
+  </si>
+  <si>
+    <t>CASE_FILE</t>
+  </si>
+  <si>
     <t>assignee, ann-acm</t>
-  </si>
-  <si>
-    <t>Complaint – Default access</t>
-  </si>
-  <si>
-    <t>participants.?[participantType == '*'].isEmpty()</t>
-  </si>
-  <si>
-    <t>*, *</t>
-  </si>
-  <si>
-    <t>Case File – Default assignee</t>
-  </si>
-  <si>
-    <t>CASE_FILE</t>
   </si>
   <si>
     <t>Case File – Default access</t>
@@ -595,7 +598,7 @@
   <dimension ref="A2:G29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -843,13 +846,13 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>37</v>
@@ -866,7 +869,7 @@
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>29</v>
@@ -875,37 +878,37 @@
         <v>30</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>34</v>
@@ -919,69 +922,69 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,10 +1028,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,30 +1039,30 @@
         <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SBI-975 - Update data access rules and assignment rules for Bactes - simlpify the addParticipantExpression function
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\1\armdev@devvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\0\armdev@devvm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>addParticipantExpression($acmObject, "$1", "$2");</t>
+  </si>
+  <si>
+    <t>Assign a participant.  First value must be the participant type, second value must be an SpEL expression that is valid when evaluated against the $acmObject.</t>
   </si>
   <si>
     <t>function Boolean evalBoolean(String expression, Object obj)
@@ -223,10 +226,7 @@
     }
     if (!found) 
     {
-      AcmParticipant ap = new AcmParticipant();
-      ap.setParticipantType(participantType);
-      ap.setParticipantLdapId(evaluated);
-      obj.getParticipants().add(ap);
+     addParticipant(obj, participantType, evaluated);
     }
 }
 function void addParticipant(AcmAssignedObject obj, String participantType, String participantId)
@@ -236,9 +236,6 @@
     ap.setParticipantLdapId(participantId);
     obj.getParticipants().add(ap);
 }</t>
-  </si>
-  <si>
-    <t>Assign a participant.  First value must be the participant type, second value must be an SpEL expression that is valid when evaluated against the $acmObject.</t>
   </si>
 </sst>
 </file>
@@ -873,8 +870,8 @@
   </sheetPr>
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1092,7 +1089,7 @@
         <v>54</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Copying the same change in config
Former-commit-id: ea633081c782ed7e86ca115b1b4a3060f74165e4
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-assignment-rules.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\0\armdev@devvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teng.wang\ACM3\acm-services\acm-service-data-access-control\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>RuleSet</t>
   </si>
@@ -236,6 +236,9 @@
     ap.setParticipantLdapId(participantId);
     obj.getParticipants().add(ap);
 }</t>
+  </si>
+  <si>
+    <t>Complaint - creator read access</t>
   </si>
 </sst>
 </file>
@@ -678,6 +681,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -713,6 +733,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -868,26 +905,26 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875"/>
-    <col min="2" max="2" width="24.33203125"/>
-    <col min="3" max="3" width="49.88671875"/>
-    <col min="4" max="4" width="81.77734375" customWidth="1"/>
-    <col min="5" max="5" width="43.88671875"/>
-    <col min="6" max="6" width="30.5546875"/>
-    <col min="7" max="7" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="21.54296875"/>
+    <col min="2" max="2" width="24.36328125"/>
+    <col min="3" max="3" width="49.90625"/>
+    <col min="4" max="4" width="81.81640625" customWidth="1"/>
+    <col min="5" max="5" width="43.90625"/>
+    <col min="6" max="6" width="30.54296875"/>
+    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.6328125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -897,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -907,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -917,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -927,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -937,7 +974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -947,7 +984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -957,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -967,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -977,7 +1014,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -987,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -997,8 +1034,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1010,7 +1047,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1032,7 +1069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1044,7 +1081,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1066,7 +1103,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1092,7 +1129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1112,7 +1149,7 @@
       </c>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
@@ -1130,7 +1167,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>32</v>
@@ -1148,7 +1185,7 @@
       </c>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>35</v>
@@ -1166,7 +1203,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>36</v>
@@ -1186,7 +1223,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>39</v>
@@ -1204,7 +1241,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>40</v>
@@ -1222,7 +1259,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>50</v>
@@ -1235,6 +1272,22 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1255,14 +1308,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625"/>
-    <col min="2" max="2" width="17.5546875"/>
-    <col min="3" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="18.6328125"/>
+    <col min="2" max="2" width="17.54296875"/>
+    <col min="3" max="1025" width="8.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1270,7 +1323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1278,7 +1331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1286,17 +1339,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1316,9 +1369,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625"/>
+    <col min="1" max="1025" width="8.6328125"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>